<commit_message>
updated experiment parameters; still need to fix readingSpacingDeg
</commit_message>
<xml_diff>
--- a/easyEyesSpreadsheets/CrowdingReadingAcuity_firstSess.xlsx
+++ b/easyEyesSpreadsheets/CrowdingReadingAcuity_firstSess.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenhu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fh986/Documents/Github/crowding-individual-difference/easyEyesSpreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6F53FA-5BAB-704F-A784-BF656B2FC899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AB56D6-B78E-B344-BB27-4C0B887116FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="29140" windowHeight="18880" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="210">
   <si>
     <t>_about</t>
   </si>
@@ -233,9 +233,6 @@
     <t>markingFixationAfterTargetOnset</t>
   </si>
   <si>
-    <t>disappear</t>
-  </si>
-  <si>
     <t>markingFixationDuringTargetBool</t>
   </si>
   <si>
@@ -266,9 +263,6 @@
     <t>markingOnsetAfterTargetOffsetSecs</t>
   </si>
   <si>
-    <t>needEasyEyesKeypadBeyondCm</t>
-  </si>
-  <si>
     <t>questionAndAnswer01</t>
   </si>
   <si>
@@ -357,9 +351,6 @@
   </si>
   <si>
     <t>responseClickedBool</t>
-  </si>
-  <si>
-    <t>responseMustClickCrosshairBool</t>
   </si>
   <si>
     <t>responseMustTrackContinuouslyBool</t>
@@ -683,6 +674,9 @@
   </si>
   <si>
     <t>_saveCursorPositionBool</t>
+  </si>
+  <si>
+    <t>typographic</t>
   </si>
 </sst>
 </file>
@@ -1177,12 +1171,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F42C05-3A7A-B849-89F1-BA0E282F9675}">
-  <dimension ref="A1:X118"/>
+  <dimension ref="A1:X116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="169" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="93" zoomScaleNormal="169" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A31" sqref="A31"/>
-      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <selection pane="topRight" activeCell="T115" sqref="T115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1204,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1292,7 +1286,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1348,7 +1342,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -1377,7 +1371,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B24" s="1" t="b">
         <v>1</v>
@@ -1464,73 +1458,73 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="M27" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="N27" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="O27" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="P27" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="W27" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="K27" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="L27" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="M27" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="N27" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="O27" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="P27" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="W27" s="4" t="s">
-        <v>197</v>
-      </c>
       <c r="X27" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
@@ -1689,64 +1683,64 @@
         <v>38</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="I31" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="J31" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="K31" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="F31" s="10" t="s">
+      <c r="L31" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="M31" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="G31" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="I31" s="17" t="s">
+      <c r="N31" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="J31" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="K31" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="L31" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="N31" s="26" t="s">
+      <c r="O31" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="O31" s="25" t="s">
+      <c r="P31" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q31" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="P31" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="T31" s="1"/>
       <c r="U31" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="3" t="s">
         <v>39</v>
       </c>
       <c r="X31" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
@@ -1884,16 +1878,16 @@
         <v>43</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K34" s="23" t="s">
         <v>43</v>
@@ -1914,22 +1908,22 @@
         <v>43</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="T34" s="1"/>
       <c r="U34" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="V34" s="1"/>
       <c r="W34" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="X34" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
@@ -2047,16 +2041,16 @@
         <v>50</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K37" s="23" t="s">
         <v>50</v>
@@ -2077,22 +2071,22 @@
         <v>50</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="T37" s="1"/>
       <c r="U37" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="V37" s="1"/>
       <c r="W37" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="X37" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
@@ -2166,11 +2160,11 @@
         <v>54</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="15"/>
@@ -2178,15 +2172,15 @@
       <c r="I40" s="15"/>
       <c r="J40" s="16"/>
       <c r="K40" s="23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L40" s="24"/>
       <c r="M40" s="23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N40" s="24"/>
       <c r="O40" s="23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="P40" s="24"/>
       <c r="Q40" s="1"/>
@@ -2203,38 +2197,38 @@
         <v>55</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="16"/>
       <c r="I41" s="15"/>
       <c r="J41" s="16"/>
       <c r="K41" s="23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L41" s="24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M41" s="23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N41" s="24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O41" s="23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P41" s="24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2250,38 +2244,38 @@
         <v>56</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="16"/>
       <c r="I42" s="15"/>
       <c r="J42" s="16"/>
       <c r="K42" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L42" s="24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M42" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N42" s="24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="O42" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P42" s="24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -2438,12 +2432,8 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
-      <c r="W45" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X45" s="4" t="b">
-        <v>1</v>
-      </c>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -2547,16 +2537,12 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
-      <c r="W48" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="X48" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="7" t="b">
         <v>1</v>
@@ -2600,34 +2586,18 @@
       <c r="P49" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="Q49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="R49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="S49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="T49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="U49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V49" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="W49" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X49" s="4" t="b">
-        <v>1</v>
-      </c>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C50" s="7">
         <v>0.15</v>
@@ -2682,49 +2652,49 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="D51" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K51" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L51" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M51" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N51" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O51" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P51" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
@@ -2737,7 +2707,7 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="7">
         <v>0.5</v>
@@ -2792,7 +2762,7 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" s="7">
         <v>0.4</v>
@@ -2847,7 +2817,7 @@
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" s="7">
         <v>1</v>
@@ -2897,16 +2867,12 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
-      <c r="W54" s="4">
-        <v>1</v>
-      </c>
-      <c r="X54" s="4">
-        <v>1</v>
-      </c>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="8"/>
@@ -2933,7 +2899,7 @@
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56" s="7">
         <v>0.05</v>
@@ -2983,16 +2949,12 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
-      <c r="W56" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="X56" s="4">
-        <v>0.03</v>
-      </c>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C57" s="7">
         <v>0.3</v>
@@ -3047,74 +3009,36 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="7"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="23"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="23"/>
+      <c r="N58" s="24"/>
+      <c r="O58" s="23"/>
+      <c r="P58" s="24"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" t="s">
+        <v>183</v>
+      </c>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="7">
-        <v>70</v>
-      </c>
-      <c r="D58" s="8">
-        <v>70</v>
-      </c>
-      <c r="E58" s="7">
-        <v>70</v>
-      </c>
-      <c r="F58" s="8">
-        <v>70</v>
-      </c>
-      <c r="G58" s="15">
-        <v>70</v>
-      </c>
-      <c r="H58" s="16">
-        <v>70</v>
-      </c>
-      <c r="I58" s="15">
-        <v>70</v>
-      </c>
-      <c r="J58" s="16">
-        <v>70</v>
-      </c>
-      <c r="K58" s="23">
-        <v>70</v>
-      </c>
-      <c r="L58" s="24">
-        <v>70</v>
-      </c>
-      <c r="M58" s="23">
-        <v>70</v>
-      </c>
-      <c r="N58" s="24">
-        <v>70</v>
-      </c>
-      <c r="O58" s="23">
-        <v>70</v>
-      </c>
-      <c r="P58" s="24">
-        <v>70</v>
-      </c>
-      <c r="Q58" s="1">
-        <v>70</v>
-      </c>
-      <c r="R58" s="1">
-        <v>70</v>
-      </c>
-      <c r="S58" s="1">
-        <v>70</v>
-      </c>
-      <c r="T58" s="1">
-        <v>70</v>
-      </c>
-      <c r="U58" s="1">
-        <v>70</v>
-      </c>
-      <c r="V58" s="1">
-        <v>70</v>
-      </c>
-      <c r="W58" s="4">
-        <v>70</v>
-      </c>
-      <c r="X58" s="4">
-        <v>70</v>
-      </c>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
@@ -3136,7 +3060,7 @@
       <c r="P59" s="24"/>
       <c r="Q59" s="1"/>
       <c r="R59" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S59" s="1"/>
       <c r="T59" s="1" t="s">
@@ -3144,7 +3068,7 @@
       </c>
       <c r="U59" s="1"/>
       <c r="V59" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="W59" s="4"/>
       <c r="X59" s="4"/>
@@ -3169,7 +3093,7 @@
       <c r="P60" s="24"/>
       <c r="Q60" s="1"/>
       <c r="R60" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="S60" s="1"/>
       <c r="T60" s="1" t="s">
@@ -3177,7 +3101,7 @@
       </c>
       <c r="U60" s="1"/>
       <c r="V60" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="W60" s="4"/>
       <c r="X60" s="4"/>
@@ -3202,7 +3126,7 @@
       <c r="P61" s="24"/>
       <c r="Q61" s="1"/>
       <c r="R61" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="S61" s="1"/>
       <c r="T61" s="1" t="s">
@@ -3210,7 +3134,7 @@
       </c>
       <c r="U61" s="1"/>
       <c r="V61" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="W61" s="4"/>
       <c r="X61" s="4"/>
@@ -3235,7 +3159,7 @@
       <c r="P62" s="24"/>
       <c r="Q62" s="1"/>
       <c r="R62" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="S62" s="1"/>
       <c r="T62" s="1" t="s">
@@ -3243,7 +3167,7 @@
       </c>
       <c r="U62" s="1"/>
       <c r="V62" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="W62" s="4"/>
       <c r="X62" s="4"/>
@@ -3266,24 +3190,28 @@
       <c r="N63" s="24"/>
       <c r="O63" s="23"/>
       <c r="P63" s="24"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" t="s">
-        <v>190</v>
-      </c>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="W63" s="4"/>
-      <c r="X63" s="4"/>
+      <c r="Q63" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="V63" s="1"/>
+      <c r="W63" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="X63" s="4" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="8"/>
@@ -3299,28 +3227,18 @@
       <c r="N64" s="24"/>
       <c r="O64" s="23"/>
       <c r="P64" s="24"/>
-      <c r="Q64" s="1" t="s">
-        <v>191</v>
-      </c>
+      <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
-      <c r="S64" s="1" t="s">
-        <v>192</v>
-      </c>
+      <c r="S64" s="1"/>
       <c r="T64" s="1"/>
-      <c r="U64" s="1" t="s">
-        <v>204</v>
-      </c>
+      <c r="U64" s="1"/>
       <c r="V64" s="1"/>
-      <c r="W64" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="X64" s="4" t="s">
-        <v>161</v>
-      </c>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
@@ -3342,12 +3260,16 @@
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
-      <c r="W65" s="4"/>
-      <c r="X65" s="4"/>
+      <c r="W65" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X65" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="8"/>
@@ -3363,18 +3285,20 @@
       <c r="N66" s="24"/>
       <c r="O66" s="23"/>
       <c r="P66" s="24"/>
-      <c r="Q66" s="1"/>
+      <c r="Q66" t="s">
+        <v>190</v>
+      </c>
       <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
+      <c r="S66" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
+      <c r="U66" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="V66" s="1"/>
-      <c r="W66" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X66" s="4" t="b">
-        <v>1</v>
-      </c>
+      <c r="W66" s="4"/>
+      <c r="X66" s="4"/>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -3394,16 +3318,16 @@
       <c r="N67" s="24"/>
       <c r="O67" s="23"/>
       <c r="P67" s="24"/>
-      <c r="Q67" t="s">
-        <v>193</v>
+      <c r="Q67" s="1">
+        <v>57</v>
       </c>
       <c r="R67" s="1"/>
-      <c r="S67" s="1" t="s">
-        <v>91</v>
+      <c r="S67" s="1">
+        <v>57</v>
       </c>
       <c r="T67" s="1"/>
-      <c r="U67" s="1" t="s">
-        <v>205</v>
+      <c r="U67" s="1">
+        <v>57</v>
       </c>
       <c r="V67" s="1"/>
       <c r="W67" s="4"/>
@@ -3411,7 +3335,7 @@
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="8"/>
@@ -3427,16 +3351,16 @@
       <c r="N68" s="24"/>
       <c r="O68" s="23"/>
       <c r="P68" s="24"/>
-      <c r="Q68" s="1">
-        <v>57</v>
+      <c r="Q68" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="R68" s="1"/>
-      <c r="S68" s="1">
-        <v>57</v>
+      <c r="S68" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="T68" s="1"/>
-      <c r="U68" s="1">
-        <v>57</v>
+      <c r="U68" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="V68" s="1"/>
       <c r="W68" s="4"/>
@@ -3472,8 +3396,12 @@
         <v>94</v>
       </c>
       <c r="V69" s="1"/>
-      <c r="W69" s="4"/>
-      <c r="X69" s="4"/>
+      <c r="W69" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="X69" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
@@ -3493,28 +3421,24 @@
       <c r="N70" s="24"/>
       <c r="O70" s="23"/>
       <c r="P70" s="24"/>
-      <c r="Q70" s="1" t="s">
-        <v>96</v>
+      <c r="Q70" s="1">
+        <v>1.2</v>
       </c>
       <c r="R70" s="1"/>
-      <c r="S70" s="1" t="s">
-        <v>96</v>
+      <c r="S70" s="1">
+        <v>1.2</v>
       </c>
       <c r="T70" s="1"/>
-      <c r="U70" s="1" t="s">
-        <v>96</v>
+      <c r="U70" s="1">
+        <v>1.2</v>
       </c>
       <c r="V70" s="1"/>
-      <c r="W70" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="X70" s="4" t="s">
-        <v>96</v>
-      </c>
+      <c r="W70" s="4"/>
+      <c r="X70" s="4"/>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="8"/>
@@ -3531,15 +3455,15 @@
       <c r="O71" s="23"/>
       <c r="P71" s="24"/>
       <c r="Q71" s="1">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="R71" s="1"/>
       <c r="S71" s="1">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="T71" s="1"/>
       <c r="U71" s="1">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="V71" s="1"/>
       <c r="W71" s="4"/>
@@ -3547,7 +3471,7 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
@@ -3564,15 +3488,15 @@
       <c r="O72" s="23"/>
       <c r="P72" s="24"/>
       <c r="Q72" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R72" s="1"/>
       <c r="S72" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T72" s="1"/>
       <c r="U72" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V72" s="1"/>
       <c r="W72" s="4"/>
@@ -3580,7 +3504,7 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="8"/>
@@ -3613,7 +3537,7 @@
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="8"/>
@@ -3630,15 +3554,15 @@
       <c r="O74" s="23"/>
       <c r="P74" s="24"/>
       <c r="Q74" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R74" s="1"/>
       <c r="S74" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T74" s="1"/>
       <c r="U74" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V74" s="1"/>
       <c r="W74" s="4"/>
@@ -3646,7 +3570,7 @@
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="8"/>
@@ -3662,20 +3586,24 @@
       <c r="N75" s="24"/>
       <c r="O75" s="23"/>
       <c r="P75" s="24"/>
-      <c r="Q75" s="1">
-        <v>5</v>
+      <c r="Q75" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="R75" s="1"/>
-      <c r="S75" s="1">
-        <v>5</v>
+      <c r="S75" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="T75" s="1"/>
-      <c r="U75" s="1">
-        <v>5</v>
+      <c r="U75" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="V75" s="1"/>
-      <c r="W75" s="4"/>
-      <c r="X75" s="4"/>
+      <c r="W75" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="X75" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -3695,28 +3623,28 @@
       <c r="N76" s="24"/>
       <c r="O76" s="23"/>
       <c r="P76" s="24"/>
-      <c r="Q76" s="1" t="s">
-        <v>103</v>
+      <c r="Q76" s="1">
+        <v>0.3</v>
       </c>
       <c r="R76" s="1"/>
-      <c r="S76" s="1" t="s">
-        <v>103</v>
+      <c r="S76" s="1">
+        <v>0.3</v>
       </c>
       <c r="T76" s="1"/>
-      <c r="U76" s="1" t="s">
-        <v>103</v>
+      <c r="U76" s="1">
+        <v>0.3</v>
       </c>
       <c r="V76" s="1"/>
-      <c r="W76" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="X76" s="4" t="s">
-        <v>103</v>
+      <c r="W76" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="X76" s="4">
+        <v>0.3</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="8"/>
@@ -3732,55 +3660,83 @@
       <c r="N77" s="24"/>
       <c r="O77" s="23"/>
       <c r="P77" s="24"/>
-      <c r="Q77" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
-      <c r="S77" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="S77" s="1"/>
       <c r="T77" s="1"/>
-      <c r="U77" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="U77" s="1"/>
       <c r="V77" s="1"/>
-      <c r="W77" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="X77" s="4">
-        <v>0.3</v>
-      </c>
+      <c r="W77" s="4"/>
+      <c r="X77" s="4"/>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C78" s="7"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="15"/>
-      <c r="H78" s="16"/>
-      <c r="I78" s="15"/>
-      <c r="J78" s="16"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="24"/>
-      <c r="M78" s="23"/>
-      <c r="N78" s="24"/>
-      <c r="O78" s="23"/>
-      <c r="P78" s="24"/>
-      <c r="Q78" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="C78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I78" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K78" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L78" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M78" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N78" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O78" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P78" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
+      <c r="S78" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="T78" s="1"/>
-      <c r="U78" s="1"/>
+      <c r="U78" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="V78" s="1"/>
-      <c r="W78" s="4"/>
-      <c r="X78" s="4"/>
+      <c r="W78" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X78" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C79" s="7" t="b">
         <v>1</v>
@@ -3824,131 +3780,119 @@
       <c r="P79" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="Q79" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
-      <c r="S79" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="S79" s="1"/>
       <c r="T79" s="1"/>
-      <c r="U79" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="U79" s="1"/>
       <c r="V79" s="1"/>
       <c r="W79" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X79" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D80" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G80" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H80" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I80" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J80" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K80" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L80" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="M80" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N80" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O80" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="P80" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q80" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C80" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="D80" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="E80" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="F80" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="G80" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="H80" s="16">
+        <v>1.25</v>
+      </c>
+      <c r="I80" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="J80" s="16">
+        <v>1.25</v>
+      </c>
+      <c r="K80" s="23">
+        <v>1.25</v>
+      </c>
+      <c r="L80" s="23">
+        <v>1.25</v>
+      </c>
+      <c r="M80" s="23">
+        <v>1.25</v>
+      </c>
+      <c r="N80" s="23">
+        <v>1.25</v>
+      </c>
+      <c r="O80" s="23">
+        <v>1.25</v>
+      </c>
+      <c r="P80" s="23">
+        <v>1.25</v>
+      </c>
+      <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
-      <c r="S80" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="S80" s="1"/>
       <c r="T80" s="1"/>
-      <c r="U80" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="U80" s="1"/>
       <c r="V80" s="1"/>
       <c r="W80" s="4"/>
       <c r="X80" s="4"/>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C81" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D81" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G81" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H81" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I81" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J81" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K81" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L81" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="M81" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N81" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O81" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="P81" s="24" t="b">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="C81" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="D81" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E81" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="F81" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="G81" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="H81" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="I81" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="J81" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="K81" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="L81" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="M81" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="N81" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="O81" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="P81" s="23">
+        <v>0.75</v>
       </c>
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
@@ -3956,58 +3900,54 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
-      <c r="W81" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="X81" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="W81" s="4"/>
+      <c r="X81" s="4"/>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C82" s="7">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="D82" s="8">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="E82" s="7">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="F82" s="8">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="G82" s="15">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="H82" s="16">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="I82" s="15">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="J82" s="16">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="K82" s="23">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="L82" s="23">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="M82" s="23">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="N82" s="23">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="O82" s="23">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="P82" s="23">
-        <v>1.25</v>
+        <v>30</v>
       </c>
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
@@ -4020,105 +3960,87 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C83" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="D83" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="E83" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="F83" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="G83" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="H83" s="16">
-        <v>0.75</v>
-      </c>
-      <c r="I83" s="15">
-        <v>0.75</v>
-      </c>
-      <c r="J83" s="16">
-        <v>0.75</v>
-      </c>
-      <c r="K83" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="L83" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="M83" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="N83" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="O83" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="P83" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="Q83" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="C83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K83" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L83" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M83" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N83" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O83" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P83" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="R83" s="1"/>
-      <c r="S83" s="1"/>
+      <c r="S83" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="T83" s="1"/>
-      <c r="U83" s="1"/>
+      <c r="U83" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="V83" s="1"/>
-      <c r="W83" s="4"/>
-      <c r="X83" s="4"/>
+      <c r="W83" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X83" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C84" s="7">
-        <v>30</v>
-      </c>
-      <c r="D84" s="8">
-        <v>30</v>
-      </c>
-      <c r="E84" s="7">
-        <v>30</v>
-      </c>
-      <c r="F84" s="8">
-        <v>30</v>
-      </c>
-      <c r="G84" s="15">
-        <v>30</v>
-      </c>
-      <c r="H84" s="16">
-        <v>30</v>
-      </c>
-      <c r="I84" s="15">
-        <v>30</v>
-      </c>
-      <c r="J84" s="16">
-        <v>30</v>
-      </c>
-      <c r="K84" s="23">
-        <v>30</v>
-      </c>
-      <c r="L84" s="23">
-        <v>30</v>
-      </c>
-      <c r="M84" s="23">
-        <v>30</v>
-      </c>
-      <c r="N84" s="23">
-        <v>30</v>
-      </c>
-      <c r="O84" s="23">
-        <v>30</v>
-      </c>
-      <c r="P84" s="23">
-        <v>30</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C84" s="7"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="23"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="23"/>
+      <c r="N84" s="24"/>
+      <c r="O84" s="23"/>
+      <c r="P84" s="24"/>
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
@@ -4130,72 +4052,38 @@
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D85" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G85" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H85" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I85" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J85" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K85" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L85" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="M85" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N85" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O85" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="P85" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q85" s="1" t="b">
-        <v>1</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C85" s="7"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="16"/>
+      <c r="K85" s="23"/>
+      <c r="L85" s="24"/>
+      <c r="M85" s="23"/>
+      <c r="N85" s="24"/>
+      <c r="O85" s="23"/>
+      <c r="P85" s="24"/>
+      <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
-      <c r="S85" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="S85" s="1"/>
       <c r="T85" s="1"/>
-      <c r="U85" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="U85" s="1"/>
       <c r="V85" s="1"/>
-      <c r="W85" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X85" s="4" t="b">
-        <v>1</v>
+      <c r="W85" s="4">
+        <v>3</v>
+      </c>
+      <c r="X85" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
@@ -4217,12 +4105,16 @@
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
-      <c r="W86" s="4"/>
-      <c r="X86" s="4"/>
+      <c r="W86" s="4">
+        <v>5</v>
+      </c>
+      <c r="X86" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="8"/>
@@ -4253,16 +4145,24 @@
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="8"/>
       <c r="E88" s="7"/>
       <c r="F88" s="8"/>
-      <c r="G88" s="15"/>
-      <c r="H88" s="16"/>
-      <c r="I88" s="15"/>
-      <c r="J88" s="16"/>
+      <c r="G88" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H88" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I88" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J88" s="16" t="s">
+        <v>115</v>
+      </c>
       <c r="K88" s="23"/>
       <c r="L88" s="24"/>
       <c r="M88" s="23"/>
@@ -4275,25 +4175,37 @@
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
       <c r="V88" s="1"/>
-      <c r="W88" s="4">
-        <v>5</v>
-      </c>
-      <c r="X88" s="4">
-        <v>5</v>
-      </c>
+      <c r="W88" s="4"/>
+      <c r="X88" s="4"/>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C89" s="7"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="15"/>
-      <c r="H89" s="16"/>
-      <c r="I89" s="15"/>
-      <c r="J89" s="16"/>
+      <c r="C89" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D89" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H89" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I89" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J89" s="16" t="b">
+        <v>0</v>
+      </c>
       <c r="K89" s="23"/>
       <c r="L89" s="24"/>
       <c r="M89" s="23"/>
@@ -4306,76 +4218,92 @@
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
       <c r="V89" s="1"/>
-      <c r="W89" s="4">
-        <v>3</v>
-      </c>
-      <c r="X89" s="4">
-        <v>3</v>
-      </c>
+      <c r="W89" s="4"/>
+      <c r="X89" s="4"/>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C90" s="7"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="H90" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I90" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="J90" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="K90" s="23"/>
-      <c r="L90" s="24"/>
-      <c r="M90" s="23"/>
-      <c r="N90" s="24"/>
-      <c r="O90" s="23"/>
-      <c r="P90" s="24"/>
-      <c r="Q90" s="1"/>
-      <c r="R90" s="1"/>
-      <c r="S90" s="1"/>
-      <c r="T90" s="1"/>
-      <c r="U90" s="1"/>
-      <c r="V90" s="1"/>
-      <c r="W90" s="4"/>
-      <c r="X90" s="4"/>
+      <c r="C90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G90" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I90" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K90" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="L90" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M90" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N90" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O90" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P90" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="R90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="S90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="T90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="U90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="V90" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="W90" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X90" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C91" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D91" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G91" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H91" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I91" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J91" s="16" t="b">
-        <v>0</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C91" s="7"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="16"/>
       <c r="K91" s="23"/>
       <c r="L91" s="24"/>
       <c r="M91" s="23"/>
@@ -4393,7 +4321,7 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="8"/>
@@ -4403,52 +4331,24 @@
       <c r="H92" s="16"/>
       <c r="I92" s="15"/>
       <c r="J92" s="16"/>
-      <c r="K92" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L92" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="M92" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="N92" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="O92" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="P92" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="R92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="S92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="T92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="U92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="W92" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="X92" s="4" t="b">
-        <v>0</v>
-      </c>
+      <c r="K92" s="23"/>
+      <c r="L92" s="24"/>
+      <c r="M92" s="23"/>
+      <c r="N92" s="24"/>
+      <c r="O92" s="23"/>
+      <c r="P92" s="24"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="W92" s="4"/>
+      <c r="X92" s="4"/>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="8"/>
@@ -4475,7 +4375,7 @@
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94" s="8"/>
@@ -4485,40 +4385,42 @@
       <c r="H94" s="16"/>
       <c r="I94" s="15"/>
       <c r="J94" s="16"/>
-      <c r="K94" s="23"/>
-      <c r="L94" s="24"/>
-      <c r="M94" s="23"/>
-      <c r="N94" s="24"/>
-      <c r="O94" s="23"/>
-      <c r="P94" s="24"/>
+      <c r="K94" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L94" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="M94" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="N94" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O94" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P94" s="24" t="b">
+        <v>0</v>
+      </c>
       <c r="Q94" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="R94" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="R94" s="1"/>
       <c r="S94" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="T94" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="T94" s="1"/>
       <c r="U94" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="V94" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="W94" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X94" s="4" t="b">
-        <v>1</v>
-      </c>
+      <c r="V94" s="1"/>
+      <c r="W94" s="4"/>
+      <c r="X94" s="4"/>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="8"/>
@@ -4545,7 +4447,7 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="8"/>
@@ -4555,35 +4457,29 @@
       <c r="H96" s="16"/>
       <c r="I96" s="15"/>
       <c r="J96" s="16"/>
-      <c r="K96" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="L96" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="M96" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="N96" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O96" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="P96" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q96" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="K96" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="L96" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="M96" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="N96" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="O96" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="P96" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
-      <c r="S96" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="S96" s="1"/>
       <c r="T96" s="1"/>
-      <c r="U96" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="U96" s="1"/>
       <c r="V96" s="1"/>
       <c r="W96" s="4"/>
       <c r="X96" s="4"/>
@@ -4600,12 +4496,24 @@
       <c r="H97" s="16"/>
       <c r="I97" s="15"/>
       <c r="J97" s="16"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="24"/>
-      <c r="M97" s="23"/>
-      <c r="N97" s="24"/>
-      <c r="O97" s="23"/>
-      <c r="P97" s="24"/>
+      <c r="K97" s="23">
+        <v>1.4</v>
+      </c>
+      <c r="L97" s="24">
+        <v>1.4</v>
+      </c>
+      <c r="M97" s="23">
+        <v>1.4</v>
+      </c>
+      <c r="N97" s="24">
+        <v>1.4</v>
+      </c>
+      <c r="O97" s="23">
+        <v>1.4</v>
+      </c>
+      <c r="P97" s="24">
+        <v>1.4</v>
+      </c>
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
@@ -4619,50 +4527,70 @@
       <c r="A98" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C98" s="7"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="15"/>
-      <c r="H98" s="16"/>
-      <c r="I98" s="15"/>
-      <c r="J98" s="16"/>
+      <c r="C98" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G98" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I98" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J98" s="16" t="s">
+        <v>127</v>
+      </c>
       <c r="K98" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L98" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M98" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="N98" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O98" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="P98" s="24" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q98" s="1" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
       <c r="R98" s="1"/>
       <c r="S98" s="1" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
       <c r="T98" s="1"/>
       <c r="U98" s="1" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
       <c r="V98" s="1"/>
-      <c r="W98" s="4"/>
-      <c r="X98" s="4"/>
+      <c r="W98" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="X98" s="4" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C99" s="7"/>
       <c r="D99" s="8"/>
@@ -4672,23 +4600,23 @@
       <c r="H99" s="16"/>
       <c r="I99" s="15"/>
       <c r="J99" s="16"/>
-      <c r="K99" s="23">
-        <v>1.4</v>
-      </c>
-      <c r="L99" s="24">
-        <v>1.4</v>
-      </c>
-      <c r="M99" s="23">
-        <v>1.4</v>
-      </c>
-      <c r="N99" s="24">
-        <v>1.4</v>
-      </c>
-      <c r="O99" s="23">
-        <v>1.4</v>
-      </c>
-      <c r="P99" s="24">
-        <v>1.4</v>
+      <c r="K99" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="L99" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="M99" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="N99" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="O99" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="P99" s="24" t="s">
+        <v>130</v>
       </c>
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
@@ -4701,384 +4629,418 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="8"/>
       <c r="E100" s="7"/>
       <c r="F100" s="8"/>
       <c r="G100" s="15" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="H100" s="16" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="I100" s="15" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="J100" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="K100" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="L100" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="M100" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="N100" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="O100" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="P100" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q100" s="1" t="s">
-        <v>131</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="K100" s="23"/>
+      <c r="L100" s="24"/>
+      <c r="M100" s="23"/>
+      <c r="N100" s="24"/>
+      <c r="O100" s="23"/>
+      <c r="P100" s="24"/>
+      <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
-      <c r="S100" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="S100" s="1"/>
       <c r="T100" s="1"/>
-      <c r="U100" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="U100" s="1"/>
       <c r="V100" s="1"/>
-      <c r="W100" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="X100" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="W100" s="4"/>
+      <c r="X100" s="4"/>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C101" s="7"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="7"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="15"/>
-      <c r="H101" s="16"/>
-      <c r="I101" s="15"/>
-      <c r="J101" s="16"/>
-      <c r="K101" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="L101" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="M101" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="N101" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="O101" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="P101" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q101" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C101" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D101" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="E101" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="F101" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G101" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H101" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="I101" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="J101" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="K101" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="L101" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="M101" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="N101" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="O101" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="P101" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
-      <c r="S101" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="S101" s="1"/>
       <c r="T101" s="1"/>
-      <c r="U101" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="U101" s="1"/>
       <c r="V101" s="1"/>
       <c r="W101" s="4"/>
       <c r="X101" s="4"/>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C102" s="7"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H102" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I102" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J102" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K102" s="23"/>
-      <c r="L102" s="24"/>
-      <c r="M102" s="23"/>
-      <c r="N102" s="24"/>
-      <c r="O102" s="23"/>
-      <c r="P102" s="24"/>
-      <c r="Q102" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="C102" s="7">
+        <v>-8</v>
+      </c>
+      <c r="D102" s="8">
+        <v>8</v>
+      </c>
+      <c r="E102" s="7">
+        <v>-8</v>
+      </c>
+      <c r="F102" s="8">
+        <v>8</v>
+      </c>
+      <c r="G102" s="15">
+        <v>-8</v>
+      </c>
+      <c r="H102" s="16">
+        <v>8</v>
+      </c>
+      <c r="I102" s="15">
+        <v>-8</v>
+      </c>
+      <c r="J102" s="16">
+        <v>8</v>
+      </c>
+      <c r="K102" s="23">
+        <v>-8</v>
+      </c>
+      <c r="L102" s="24">
+        <v>8</v>
+      </c>
+      <c r="M102" s="23">
+        <v>-8</v>
+      </c>
+      <c r="N102" s="24">
+        <v>8</v>
+      </c>
+      <c r="O102" s="23">
+        <v>-8</v>
+      </c>
+      <c r="P102" s="24">
+        <v>8</v>
+      </c>
+      <c r="Q102" s="1">
+        <v>0</v>
+      </c>
       <c r="R102" s="1"/>
-      <c r="S102" s="1"/>
+      <c r="S102" s="1">
+        <v>0</v>
+      </c>
       <c r="T102" s="1"/>
-      <c r="U102" s="1"/>
+      <c r="U102" s="1">
+        <v>0</v>
+      </c>
       <c r="V102" s="1"/>
-      <c r="W102" s="4"/>
-      <c r="X102" s="4"/>
+      <c r="W102" s="4">
+        <v>0</v>
+      </c>
+      <c r="X102" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C103" s="7">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D103" s="8">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E103" s="7">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F103" s="8">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G103" s="15">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H103" s="16">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I103" s="15">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J103" s="16">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="K103" s="23">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="L103" s="24">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="M103" s="23">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="N103" s="24">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="O103" s="23">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="P103" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="Q103" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q103" s="1">
+        <v>0</v>
+      </c>
       <c r="R103" s="1"/>
-      <c r="S103" s="1"/>
+      <c r="S103" s="1">
+        <v>0</v>
+      </c>
       <c r="T103" s="1"/>
-      <c r="U103" s="1"/>
+      <c r="U103" s="1">
+        <v>0</v>
+      </c>
       <c r="V103" s="1"/>
-      <c r="W103" s="4"/>
-      <c r="X103" s="4"/>
+      <c r="W103" s="4">
+        <v>0</v>
+      </c>
+      <c r="X103" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C104" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C104" s="7">
-        <v>-8</v>
-      </c>
-      <c r="D104" s="8">
-        <v>8</v>
-      </c>
-      <c r="E104" s="7">
-        <v>-8</v>
-      </c>
-      <c r="F104" s="8">
-        <v>8</v>
-      </c>
-      <c r="G104" s="15">
-        <v>-8</v>
-      </c>
-      <c r="H104" s="16">
-        <v>8</v>
-      </c>
-      <c r="I104" s="15">
-        <v>-8</v>
-      </c>
-      <c r="J104" s="16">
-        <v>8</v>
-      </c>
-      <c r="K104" s="23">
-        <v>-8</v>
-      </c>
-      <c r="L104" s="24">
-        <v>8</v>
-      </c>
-      <c r="M104" s="23">
-        <v>-8</v>
-      </c>
-      <c r="N104" s="24">
-        <v>8</v>
-      </c>
-      <c r="O104" s="23">
-        <v>-8</v>
-      </c>
-      <c r="P104" s="24">
-        <v>8</v>
-      </c>
-      <c r="Q104" s="1">
-        <v>0</v>
+      <c r="D104" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F104" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G104" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H104" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="I104" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="J104" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="K104" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="L104" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="M104" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="N104" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="O104" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="P104" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q104" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="R104" s="1"/>
-      <c r="S104" s="1">
-        <v>0</v>
+      <c r="S104" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="T104" s="1"/>
-      <c r="U104" s="1">
-        <v>0</v>
+      <c r="U104" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="V104" s="1"/>
-      <c r="W104" s="4">
-        <v>0</v>
-      </c>
-      <c r="X104" s="4">
-        <v>0</v>
+      <c r="W104" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="X104" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C105" s="7">
-        <v>0</v>
-      </c>
-      <c r="D105" s="8">
-        <v>0</v>
-      </c>
-      <c r="E105" s="7">
-        <v>0</v>
-      </c>
-      <c r="F105" s="8">
-        <v>0</v>
-      </c>
-      <c r="G105" s="15">
-        <v>0</v>
-      </c>
-      <c r="H105" s="16">
-        <v>0</v>
-      </c>
-      <c r="I105" s="15">
-        <v>0</v>
-      </c>
-      <c r="J105" s="16">
-        <v>0</v>
-      </c>
-      <c r="K105" s="23">
-        <v>0</v>
-      </c>
-      <c r="L105" s="24">
-        <v>0</v>
-      </c>
-      <c r="M105" s="23">
-        <v>0</v>
-      </c>
-      <c r="N105" s="24">
-        <v>0</v>
-      </c>
-      <c r="O105" s="23">
-        <v>0</v>
-      </c>
-      <c r="P105" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q105" s="1">
+        <v>140</v>
+      </c>
+      <c r="C105" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D105" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G105" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J105" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K105" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L105" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="M105" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="N105" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O105" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P105" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="1" t="b">
         <v>0</v>
       </c>
       <c r="R105" s="1"/>
-      <c r="S105" s="1">
+      <c r="S105" s="1" t="b">
         <v>0</v>
       </c>
       <c r="T105" s="1"/>
-      <c r="U105" s="1">
+      <c r="U105" s="1" t="b">
         <v>0</v>
       </c>
       <c r="V105" s="1"/>
-      <c r="W105" s="4">
-        <v>0</v>
-      </c>
-      <c r="X105" s="4">
+      <c r="W105" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X105" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G106" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H106" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I106" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J106" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K106" s="23" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="L106" s="24" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="M106" s="23" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="N106" s="24" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="O106" s="23" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="P106" s="24" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="R106" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="S106" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="T106" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="T106" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="U106" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="V106" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="V106" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="W106" s="4" t="s">
         <v>142</v>
       </c>
@@ -5088,284 +5050,234 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C107" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D107" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F107" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G107" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H107" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I107" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J107" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K107" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="L107" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="M107" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="N107" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O107" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="P107" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q107" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="R107" s="1"/>
-      <c r="S107" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="T107" s="1"/>
-      <c r="U107" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="V107" s="1"/>
-      <c r="W107" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="X107" s="4" t="b">
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="C107" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="D107" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="E107" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="F107" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="G107" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="H107" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="I107" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="J107" s="16">
+        <v>1.4</v>
+      </c>
+      <c r="K107" s="23">
+        <v>1.4</v>
+      </c>
+      <c r="L107" s="24">
+        <v>1.4</v>
+      </c>
+      <c r="M107" s="23">
+        <v>1.4</v>
+      </c>
+      <c r="N107" s="24">
+        <v>1.4</v>
+      </c>
+      <c r="O107" s="23">
+        <v>1.4</v>
+      </c>
+      <c r="P107" s="24">
+        <v>1.4</v>
+      </c>
+      <c r="Q107" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="R107" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="S107" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="T107" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="U107" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="V107" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="W107" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="X107" s="4">
+        <v>1.4</v>
       </c>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C108" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F108" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G108" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="H108" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="I108" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="J108" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="K108" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="L108" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="M108" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="N108" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="O108" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="P108" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R108" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="S108" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="T108" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="U108" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="V108" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="W108" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="X108" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="C108" s="7"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="15"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="15"/>
+      <c r="J108" s="16"/>
+      <c r="K108" s="23"/>
+      <c r="L108" s="24"/>
+      <c r="M108" s="23"/>
+      <c r="N108" s="24"/>
+      <c r="O108" s="23"/>
+      <c r="P108" s="24"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+      <c r="S108" s="1"/>
+      <c r="T108" s="1"/>
+      <c r="U108" s="1"/>
+      <c r="V108" s="1"/>
+      <c r="W108" s="4"/>
+      <c r="X108" s="4"/>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>208</v>
+        <v>145</v>
       </c>
       <c r="C109" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="D109" s="8">
-        <v>1.4</v>
+        <v>0.01</v>
+      </c>
+      <c r="D109" s="7">
+        <v>0.01</v>
       </c>
       <c r="E109" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="F109" s="8">
-        <v>1.4</v>
+        <v>0.01</v>
+      </c>
+      <c r="F109" s="7">
+        <v>0.01</v>
       </c>
       <c r="G109" s="15">
-        <v>1.4</v>
-      </c>
-      <c r="H109" s="16">
-        <v>1.4</v>
+        <v>0.01</v>
+      </c>
+      <c r="H109" s="15">
+        <v>0.01</v>
       </c>
       <c r="I109" s="15">
-        <v>1.4</v>
-      </c>
-      <c r="J109" s="16">
-        <v>1.4</v>
+        <v>0.01</v>
+      </c>
+      <c r="J109" s="15">
+        <v>0.01</v>
       </c>
       <c r="K109" s="23">
-        <v>1.4</v>
+        <v>0.01</v>
       </c>
       <c r="L109" s="24">
-        <v>1.4</v>
+        <v>0.01</v>
       </c>
       <c r="M109" s="23">
-        <v>1.4</v>
+        <v>0.01</v>
       </c>
       <c r="N109" s="24">
-        <v>1.4</v>
+        <v>0.01</v>
       </c>
       <c r="O109" s="23">
-        <v>1.4</v>
+        <v>0.01</v>
       </c>
       <c r="P109" s="24">
-        <v>1.4</v>
-      </c>
-      <c r="Q109" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="R109" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="S109" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="T109" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="U109" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="V109" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="W109" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="X109" s="4">
-        <v>1.4</v>
-      </c>
+        <v>0.01</v>
+      </c>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+      <c r="S109" s="1"/>
+      <c r="T109" s="1"/>
+      <c r="U109" s="1"/>
+      <c r="V109" s="1"/>
+      <c r="W109" s="4"/>
+      <c r="X109" s="4"/>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C110" s="7"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="7"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="15"/>
-      <c r="H110" s="16"/>
-      <c r="I110" s="15"/>
-      <c r="J110" s="16"/>
-      <c r="K110" s="23"/>
-      <c r="L110" s="24"/>
-      <c r="M110" s="23"/>
-      <c r="N110" s="24"/>
-      <c r="O110" s="23"/>
-      <c r="P110" s="24"/>
+        <v>146</v>
+      </c>
+      <c r="C110" s="7">
+        <v>4</v>
+      </c>
+      <c r="D110" s="8">
+        <v>4</v>
+      </c>
+      <c r="E110" s="7">
+        <v>4</v>
+      </c>
+      <c r="F110" s="8">
+        <v>4</v>
+      </c>
+      <c r="G110" s="15">
+        <v>4</v>
+      </c>
+      <c r="H110" s="16">
+        <v>4</v>
+      </c>
+      <c r="I110" s="15">
+        <v>4</v>
+      </c>
+      <c r="J110" s="16">
+        <v>4</v>
+      </c>
+      <c r="K110" s="23">
+        <v>2</v>
+      </c>
+      <c r="L110" s="24">
+        <v>2</v>
+      </c>
+      <c r="M110" s="23">
+        <v>2</v>
+      </c>
+      <c r="N110" s="24">
+        <v>2</v>
+      </c>
+      <c r="O110" s="23">
+        <v>2</v>
+      </c>
+      <c r="P110" s="24">
+        <v>2</v>
+      </c>
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
       <c r="S110" s="1"/>
       <c r="T110" s="1"/>
       <c r="U110" s="1"/>
       <c r="V110" s="1"/>
-      <c r="W110" s="4"/>
-      <c r="X110" s="4"/>
+      <c r="W110" s="4">
+        <v>2</v>
+      </c>
+      <c r="X110" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C111" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="D111" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="E111" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="F111" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="G111" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="H111" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="I111" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="J111" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="K111" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="L111" s="24">
-        <v>0.01</v>
-      </c>
-      <c r="M111" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="N111" s="24">
-        <v>0.01</v>
-      </c>
-      <c r="O111" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="P111" s="24">
-        <v>0.01</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C111" s="7"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="15"/>
+      <c r="J111" s="16"/>
+      <c r="K111" s="23"/>
+      <c r="L111" s="24"/>
+      <c r="M111" s="23"/>
+      <c r="N111" s="24"/>
+      <c r="O111" s="23"/>
+      <c r="P111" s="24"/>
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
       <c r="S111" s="1"/>
@@ -5377,49 +5289,49 @@
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C112" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C112" s="7">
-        <v>4</v>
-      </c>
-      <c r="D112" s="8">
-        <v>4</v>
-      </c>
-      <c r="E112" s="7">
-        <v>4</v>
-      </c>
-      <c r="F112" s="8">
-        <v>4</v>
-      </c>
-      <c r="G112" s="15">
-        <v>4</v>
-      </c>
-      <c r="H112" s="16">
-        <v>4</v>
-      </c>
-      <c r="I112" s="15">
-        <v>4</v>
-      </c>
-      <c r="J112" s="16">
-        <v>4</v>
-      </c>
-      <c r="K112" s="23">
-        <v>2</v>
-      </c>
-      <c r="L112" s="24">
-        <v>2</v>
-      </c>
-      <c r="M112" s="23">
-        <v>2</v>
-      </c>
-      <c r="N112" s="24">
-        <v>2</v>
-      </c>
-      <c r="O112" s="23">
-        <v>2</v>
-      </c>
-      <c r="P112" s="24">
-        <v>2</v>
+      <c r="D112" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G112" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H112" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="I112" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="J112" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="K112" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="L112" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="M112" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="N112" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="O112" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="P112" s="24" t="s">
+        <v>101</v>
       </c>
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
@@ -5427,25 +5339,41 @@
       <c r="T112" s="1"/>
       <c r="U112" s="1"/>
       <c r="V112" s="1"/>
-      <c r="W112" s="4">
-        <v>2</v>
-      </c>
-      <c r="X112" s="4">
-        <v>2</v>
+      <c r="W112" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="X112" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C113" s="7"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="15"/>
-      <c r="H113" s="16"/>
-      <c r="I113" s="15"/>
-      <c r="J113" s="16"/>
+        <v>151</v>
+      </c>
+      <c r="C113" s="7">
+        <v>10</v>
+      </c>
+      <c r="D113" s="8">
+        <v>10</v>
+      </c>
+      <c r="E113" s="7">
+        <v>10</v>
+      </c>
+      <c r="F113" s="8">
+        <v>10</v>
+      </c>
+      <c r="G113" s="15">
+        <v>5</v>
+      </c>
+      <c r="H113" s="16">
+        <v>5</v>
+      </c>
+      <c r="I113" s="15">
+        <v>5</v>
+      </c>
+      <c r="J113" s="16">
+        <v>5</v>
+      </c>
       <c r="K113" s="23"/>
       <c r="L113" s="24"/>
       <c r="M113" s="23"/>
@@ -5458,54 +5386,58 @@
       <c r="T113" s="1"/>
       <c r="U113" s="1"/>
       <c r="V113" s="1"/>
-      <c r="W113" s="4"/>
-      <c r="X113" s="4"/>
+      <c r="W113" s="4">
+        <v>8</v>
+      </c>
+      <c r="X113" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C114" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D114" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E114" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="G114" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="H114" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="I114" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="J114" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="K114" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="L114" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="M114" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="N114" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="O114" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="P114" s="24" t="s">
-        <v>103</v>
+      <c r="C114" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="D114" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="E114" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="F114" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="G114" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="H114" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="I114" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="J114" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="K114" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="L114" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="M114" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="N114" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="O114" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="P114" s="24">
+        <v>0.7</v>
       </c>
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
@@ -5513,47 +5445,59 @@
       <c r="T114" s="1"/>
       <c r="U114" s="1"/>
       <c r="V114" s="1"/>
-      <c r="W114" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="X114" s="4" t="s">
-        <v>135</v>
+      <c r="W114" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="X114" s="4">
+        <v>0.7</v>
       </c>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C115" s="7">
-        <v>10</v>
+        <v>1.2</v>
       </c>
       <c r="D115" s="8">
-        <v>10</v>
+        <v>1.2</v>
       </c>
       <c r="E115" s="7">
-        <v>10</v>
+        <v>1.2</v>
       </c>
       <c r="F115" s="8">
-        <v>10</v>
+        <v>1.2</v>
       </c>
       <c r="G115" s="15">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="H115" s="16">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="I115" s="15">
-        <v>5</v>
+        <v>1.2</v>
       </c>
       <c r="J115" s="16">
-        <v>5</v>
-      </c>
-      <c r="K115" s="23"/>
-      <c r="L115" s="24"/>
-      <c r="M115" s="23"/>
-      <c r="N115" s="24"/>
-      <c r="O115" s="23"/>
-      <c r="P115" s="24"/>
+        <v>1.2</v>
+      </c>
+      <c r="K115" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="L115" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="M115" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="N115" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="O115" s="23">
+        <v>1.2</v>
+      </c>
+      <c r="P115" s="23">
+        <v>1.2</v>
+      </c>
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
       <c r="S115" s="1"/>
@@ -5561,192 +5505,74 @@
       <c r="U115" s="1"/>
       <c r="V115" s="1"/>
       <c r="W115" s="4">
-        <v>8</v>
+        <v>1.2</v>
       </c>
       <c r="X115" s="4">
-        <v>8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C116" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="D116" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="E116" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="F116" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="G116" s="15">
-        <v>0.7</v>
-      </c>
-      <c r="H116" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="I116" s="15">
-        <v>0.7</v>
-      </c>
-      <c r="J116" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="K116" s="23">
-        <v>0.7</v>
-      </c>
-      <c r="L116" s="24">
-        <v>0.7</v>
-      </c>
-      <c r="M116" s="23">
-        <v>0.7</v>
-      </c>
-      <c r="N116" s="24">
-        <v>0.7</v>
-      </c>
-      <c r="O116" s="23">
-        <v>0.7</v>
-      </c>
-      <c r="P116" s="24">
-        <v>0.7</v>
-      </c>
-      <c r="Q116" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="C116" s="11">
+        <v>40</v>
+      </c>
+      <c r="D116" s="12">
+        <v>40</v>
+      </c>
+      <c r="E116" s="11">
+        <v>40</v>
+      </c>
+      <c r="F116" s="12">
+        <v>40</v>
+      </c>
+      <c r="G116" s="19">
+        <v>40</v>
+      </c>
+      <c r="H116" s="20">
+        <v>40</v>
+      </c>
+      <c r="I116" s="19">
+        <v>40</v>
+      </c>
+      <c r="J116" s="20">
+        <v>40</v>
+      </c>
+      <c r="K116" s="27">
+        <v>40</v>
+      </c>
+      <c r="L116" s="28">
+        <v>40</v>
+      </c>
+      <c r="M116" s="27">
+        <v>40</v>
+      </c>
+      <c r="N116" s="28">
+        <v>40</v>
+      </c>
+      <c r="O116" s="27">
+        <v>40</v>
+      </c>
+      <c r="P116" s="28">
+        <v>40</v>
+      </c>
+      <c r="Q116" s="1">
+        <v>40</v>
+      </c>
       <c r="R116" s="1"/>
-      <c r="S116" s="1"/>
+      <c r="S116" s="1">
+        <v>40</v>
+      </c>
       <c r="T116" s="1"/>
-      <c r="U116" s="1"/>
+      <c r="U116" s="1">
+        <v>40</v>
+      </c>
       <c r="V116" s="1"/>
       <c r="W116" s="4">
-        <v>0.7</v>
+        <v>40</v>
       </c>
       <c r="X116" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C117" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="D117" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="E117" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="F117" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="G117" s="15">
-        <v>1.2</v>
-      </c>
-      <c r="H117" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="I117" s="15">
-        <v>1.2</v>
-      </c>
-      <c r="J117" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="K117" s="23">
-        <v>1.2</v>
-      </c>
-      <c r="L117" s="23">
-        <v>1.2</v>
-      </c>
-      <c r="M117" s="23">
-        <v>1.2</v>
-      </c>
-      <c r="N117" s="23">
-        <v>1.2</v>
-      </c>
-      <c r="O117" s="23">
-        <v>1.2</v>
-      </c>
-      <c r="P117" s="23">
-        <v>1.2</v>
-      </c>
-      <c r="Q117" s="1"/>
-      <c r="R117" s="1"/>
-      <c r="S117" s="1"/>
-      <c r="T117" s="1"/>
-      <c r="U117" s="1"/>
-      <c r="V117" s="1"/>
-      <c r="W117" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="X117" s="4">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C118" s="11">
-        <v>40</v>
-      </c>
-      <c r="D118" s="12">
-        <v>40</v>
-      </c>
-      <c r="E118" s="11">
-        <v>40</v>
-      </c>
-      <c r="F118" s="12">
-        <v>40</v>
-      </c>
-      <c r="G118" s="19">
-        <v>40</v>
-      </c>
-      <c r="H118" s="20">
-        <v>40</v>
-      </c>
-      <c r="I118" s="19">
-        <v>40</v>
-      </c>
-      <c r="J118" s="20">
-        <v>40</v>
-      </c>
-      <c r="K118" s="27">
-        <v>40</v>
-      </c>
-      <c r="L118" s="28">
-        <v>40</v>
-      </c>
-      <c r="M118" s="27">
-        <v>40</v>
-      </c>
-      <c r="N118" s="28">
-        <v>40</v>
-      </c>
-      <c r="O118" s="27">
-        <v>40</v>
-      </c>
-      <c r="P118" s="28">
-        <v>40</v>
-      </c>
-      <c r="Q118" s="1">
-        <v>40</v>
-      </c>
-      <c r="R118" s="1"/>
-      <c r="S118" s="1">
-        <v>40</v>
-      </c>
-      <c r="T118" s="1"/>
-      <c r="U118" s="1">
-        <v>40</v>
-      </c>
-      <c r="V118" s="1"/>
-      <c r="W118" s="4">
-        <v>40</v>
-      </c>
-      <c r="X118" s="4">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated reading fontsize parameters, fixed bugs
</commit_message>
<xml_diff>
--- a/easyEyesSpreadsheets/CrowdingReadingAcuity_firstSess.xlsx
+++ b/easyEyesSpreadsheets/CrowdingReadingAcuity_firstSess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fh986/Documents/Github/crowding-individual-difference/easyEyesSpreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AB56D6-B78E-B344-BB27-4C0B887116FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BF3C09-5044-CC4C-8810-D60311FF39AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1173,10 +1173,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F42C05-3A7A-B849-89F1-BA0E282F9675}">
   <dimension ref="A1:X116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="93" zoomScaleNormal="169" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="93" zoomScaleNormal="169" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A31" sqref="A31"/>
-      <selection pane="topRight" activeCell="T115" sqref="T115"/>
+      <selection pane="topRight" activeCell="X76" sqref="X76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3624,22 +3624,22 @@
       <c r="O76" s="23"/>
       <c r="P76" s="24"/>
       <c r="Q76" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="R76" s="1"/>
       <c r="S76" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T76" s="1"/>
       <c r="U76" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="V76" s="1"/>
       <c r="W76" s="4">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="X76" s="4">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated language and targetTask to match the latest EE updates
</commit_message>
<xml_diff>
--- a/easyEyesSpreadsheets/CrowdingReadingAcuity_firstSess.xlsx
+++ b/easyEyesSpreadsheets/CrowdingReadingAcuity_firstSess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenhu/Documents/GitHub/crowding-individual-difference/easyEyesSpreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767F00AF-AE26-3D43-BC1F-3A30B2452F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AB6197-55CA-3D48-9B8D-A3399E62CD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="760" windowWidth="29180" windowHeight="18880" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
+    <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" xr2:uid="{F1A85D42-BFAE-944F-85F3-75B22481207D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="212">
   <si>
     <t>_about</t>
   </si>
@@ -59,9 +59,6 @@
     <t>_language</t>
   </si>
   <si>
-    <t>English (US)</t>
-  </si>
-  <si>
     <t>_languageSelectionByParticipantBool</t>
   </si>
   <si>
@@ -462,9 +459,6 @@
   </si>
   <si>
     <t>identify</t>
-  </si>
-  <si>
-    <t>questionAndAnswer</t>
   </si>
   <si>
     <t>thresholdBeta</t>
@@ -687,6 +681,9 @@
   </si>
   <si>
     <t>blindspot</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -1186,10 +1183,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F42C05-3A7A-B849-89F1-BA0E282F9675}">
   <dimension ref="A1:X117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="169" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="166" zoomScaleNormal="169" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection activeCell="A31" sqref="A31"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="V107" sqref="V107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1203,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1211,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1235,12 +1232,12 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="b">
         <v>1</v>
@@ -1248,7 +1245,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>0</v>
@@ -1256,23 +1253,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>6</v>
@@ -1280,31 +1277,31 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
         <v>60</v>
@@ -1312,7 +1309,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -1320,15 +1317,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>15</v>
@@ -1336,7 +1333,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="b">
         <v>0</v>
@@ -1344,7 +1341,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="b">
         <v>0</v>
@@ -1352,39 +1349,39 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" s="1" t="b">
         <v>1</v>
@@ -1392,7 +1389,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="b">
         <v>1</v>
@@ -1400,7 +1397,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -1471,78 +1468,78 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K27" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="L27" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="M27" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="N27" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="O27" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="P27" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="W27" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="X27" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K27" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="L27" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="M27" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="N27" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="O27" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="P27" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="V27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="W27" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="X27" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="7" t="b">
         <v>1</v>
@@ -1607,72 +1604,72 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K29" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L29" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N29" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="O29" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P29" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="T29" s="1"/>
       <c r="U29" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="X29" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="7" t="b">
         <v>1</v>
@@ -1731,7 +1728,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
@@ -1758,72 +1755,72 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="H32" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="I32" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="J32" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="K32" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="L32" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="M32" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="J32" s="18" t="s">
+      <c r="N32" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="K32" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="L32" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="M32" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="N32" s="26" t="s">
-        <v>174</v>
-      </c>
       <c r="O32" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P32" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q32" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="T32" s="1"/>
       <c r="U32" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="V32" s="1"/>
       <c r="W32" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
@@ -1882,7 +1879,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="7">
         <v>10</v>
@@ -1941,137 +1938,137 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="D35" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L35" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M35" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N35" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O35" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="V35" s="1"/>
       <c r="W35" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="H36" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="I36" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="J36" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="K36" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="L36" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="N36" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="O36" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="P36" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q36" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="K36" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="L36" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="M36" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="N36" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="O36" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="P36" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T36" s="1"/>
       <c r="U36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V36" s="1"/>
       <c r="W36" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="X36" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="8"/>
@@ -2104,88 +2101,88 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="D38" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L38" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M38" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N38" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O38" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P38" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R38" s="1"/>
       <c r="S38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T38" s="1"/>
       <c r="U38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V38" s="1"/>
       <c r="W38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
       <c r="G39" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K39" s="23"/>
       <c r="L39" s="24"/>
@@ -2204,7 +2201,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
@@ -2235,14 +2232,14 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="15"/>
@@ -2250,15 +2247,15 @@
       <c r="I41" s="15"/>
       <c r="J41" s="16"/>
       <c r="K41" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L41" s="24"/>
       <c r="M41" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N41" s="24"/>
       <c r="O41" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="P41" s="24"/>
       <c r="Q41" s="1"/>
@@ -2272,41 +2269,41 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="16"/>
       <c r="I42" s="15"/>
       <c r="J42" s="16"/>
       <c r="K42" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L42" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M42" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="N42" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O42" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="P42" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -2319,41 +2316,41 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="16"/>
       <c r="I43" s="15"/>
       <c r="J43" s="16"/>
       <c r="K43" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L43" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M43" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N43" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O43" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P43" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -2366,49 +2363,49 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="D44" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="H44" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="I44" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="J44" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G44" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>58</v>
-      </c>
       <c r="K44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P44" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -2421,7 +2418,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="7">
         <v>-0.25</v>
@@ -2476,7 +2473,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="8"/>
@@ -2515,7 +2512,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="7">
         <v>2</v>
@@ -2558,23 +2555,23 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="8"/>
       <c r="E48" s="7"/>
       <c r="F48" s="8"/>
       <c r="G48" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K48" s="23"/>
       <c r="L48" s="24"/>
@@ -2593,7 +2590,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="8"/>
@@ -2620,7 +2617,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="7" t="b">
         <v>1</v>
@@ -2675,7 +2672,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="7">
         <v>0.15</v>
@@ -2730,49 +2727,49 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="D52" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K52" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L52" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M52" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N52" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O52" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P52" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
@@ -2785,7 +2782,7 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C53" s="7">
         <v>0.5</v>
@@ -2840,7 +2837,7 @@
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C54" s="7">
         <v>0.4</v>
@@ -2895,7 +2892,7 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55" s="7">
         <v>1</v>
@@ -2950,7 +2947,7 @@
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="8"/>
@@ -2977,7 +2974,7 @@
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C57" s="7">
         <v>0.05</v>
@@ -3032,7 +3029,7 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C58" s="7">
         <v>0.3</v>
@@ -3087,7 +3084,7 @@
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="8"/>
@@ -3105,22 +3102,22 @@
       <c r="P59" s="24"/>
       <c r="Q59" s="1"/>
       <c r="R59" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="S59" s="1"/>
       <c r="T59" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U59" s="1"/>
       <c r="V59" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="W59" s="4"/>
       <c r="X59" s="4"/>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="8"/>
@@ -3138,22 +3135,22 @@
       <c r="P60" s="24"/>
       <c r="Q60" s="1"/>
       <c r="R60" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="S60" s="1"/>
       <c r="T60" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U60" s="1"/>
       <c r="V60" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="W60" s="4"/>
       <c r="X60" s="4"/>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="8"/>
@@ -3171,22 +3168,22 @@
       <c r="P61" s="24"/>
       <c r="Q61" s="1"/>
       <c r="R61" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="S61" s="1"/>
       <c r="T61" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U61" s="1"/>
       <c r="V61" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="W61" s="4"/>
       <c r="X61" s="4"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="8"/>
@@ -3204,22 +3201,22 @@
       <c r="P62" s="24"/>
       <c r="Q62" s="1"/>
       <c r="R62" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="S62" s="1"/>
       <c r="T62" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U62" s="1"/>
       <c r="V62" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="W62" s="4"/>
       <c r="X62" s="4"/>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="8"/>
@@ -3237,22 +3234,22 @@
       <c r="P63" s="24"/>
       <c r="Q63" s="1"/>
       <c r="R63" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="S63" s="1"/>
       <c r="T63" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U63" s="1"/>
       <c r="V63" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="W63" s="4"/>
       <c r="X63" s="4"/>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="8"/>
@@ -3269,27 +3266,27 @@
       <c r="O64" s="23"/>
       <c r="P64" s="24"/>
       <c r="Q64" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="R64" s="1"/>
       <c r="S64" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="T64" s="1"/>
       <c r="U64" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="V64" s="1"/>
       <c r="W64" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="X64" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="8"/>
@@ -3316,7 +3313,7 @@
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="8"/>
@@ -3347,7 +3344,7 @@
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="8"/>
@@ -3364,15 +3361,15 @@
       <c r="O67" s="23"/>
       <c r="P67" s="24"/>
       <c r="Q67" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R67" s="1"/>
       <c r="S67" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="V67" s="1"/>
       <c r="W67" s="4"/>
@@ -3380,7 +3377,7 @@
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="8"/>
@@ -3413,7 +3410,7 @@
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="8"/>
@@ -3430,15 +3427,15 @@
       <c r="O69" s="23"/>
       <c r="P69" s="24"/>
       <c r="Q69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R69" s="1"/>
       <c r="S69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T69" s="1"/>
       <c r="U69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V69" s="1"/>
       <c r="W69" s="4"/>
@@ -3446,7 +3443,7 @@
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="8"/>
@@ -3463,27 +3460,27 @@
       <c r="O70" s="23"/>
       <c r="P70" s="24"/>
       <c r="Q70" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R70" s="1"/>
       <c r="S70" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T70" s="1"/>
       <c r="U70" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V70" s="1"/>
       <c r="W70" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X70" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="8"/>
@@ -3516,7 +3513,7 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
@@ -3549,7 +3546,7 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="8"/>
@@ -3582,7 +3579,7 @@
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="8"/>
@@ -3615,7 +3612,7 @@
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="8"/>
@@ -3648,7 +3645,7 @@
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="8"/>
@@ -3665,27 +3662,27 @@
       <c r="O76" s="23"/>
       <c r="P76" s="24"/>
       <c r="Q76" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R76" s="1"/>
       <c r="S76" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T76" s="1"/>
       <c r="U76" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V76" s="1"/>
       <c r="W76" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X76" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="8"/>
@@ -3722,7 +3719,7 @@
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="8"/>
@@ -3749,7 +3746,7 @@
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C79" s="7" t="b">
         <v>1</v>
@@ -3814,7 +3811,7 @@
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C80" s="7" t="b">
         <v>1</v>
@@ -3873,7 +3870,7 @@
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C81" s="7">
         <v>1.25</v>
@@ -3928,7 +3925,7 @@
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C82" s="7">
         <v>0.75</v>
@@ -3983,7 +3980,7 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C83" s="7">
         <v>30</v>
@@ -4038,7 +4035,7 @@
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C84" s="7" t="b">
         <v>1</v>
@@ -4103,7 +4100,7 @@
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="8"/>
@@ -4130,7 +4127,7 @@
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
@@ -4161,7 +4158,7 @@
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="8"/>
@@ -4192,7 +4189,7 @@
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="8"/>
@@ -4223,23 +4220,23 @@
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="8"/>
       <c r="E89" s="7"/>
       <c r="F89" s="8"/>
       <c r="G89" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H89" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I89" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J89" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K89" s="23"/>
       <c r="L89" s="24"/>
@@ -4258,7 +4255,7 @@
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C90" s="7" t="b">
         <v>0</v>
@@ -4301,7 +4298,7 @@
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C91" s="7" t="b">
         <v>1</v>
@@ -4372,7 +4369,7 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="8"/>
@@ -4399,7 +4396,7 @@
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="8"/>
@@ -4426,7 +4423,7 @@
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94" s="8"/>
@@ -4453,7 +4450,7 @@
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="8"/>
@@ -4498,7 +4495,7 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="8"/>
@@ -4525,7 +4522,7 @@
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="8"/>
@@ -4536,22 +4533,22 @@
       <c r="I97" s="15"/>
       <c r="J97" s="16"/>
       <c r="K97" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L97" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M97" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N97" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O97" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P97" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
@@ -4564,7 +4561,7 @@
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="8"/>
@@ -4603,72 +4600,72 @@
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F99" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G99" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C99" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G99" s="15" t="s">
+      <c r="H99" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="I99" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J99" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="K99" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="H99" s="16" t="s">
+      <c r="L99" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="I99" s="15" t="s">
+      <c r="M99" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="J99" s="16" t="s">
+      <c r="N99" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="K99" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="L99" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="M99" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="N99" s="24" t="s">
-        <v>127</v>
-      </c>
       <c r="O99" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P99" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R99" s="1"/>
       <c r="S99" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="T99" s="1"/>
       <c r="U99" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="V99" s="1"/>
       <c r="W99" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="X99" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="8"/>
@@ -4679,22 +4676,22 @@
       <c r="I100" s="15"/>
       <c r="J100" s="16"/>
       <c r="K100" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L100" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M100" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N100" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O100" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P100" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
@@ -4707,23 +4704,23 @@
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="8"/>
       <c r="E101" s="7"/>
       <c r="F101" s="8"/>
       <c r="G101" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H101" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I101" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J101" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K101" s="23"/>
       <c r="L101" s="24"/>
@@ -4742,7 +4739,7 @@
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C102" s="7">
         <v>0.15</v>
@@ -4797,7 +4794,7 @@
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C103" s="7">
         <v>-8</v>
@@ -4862,7 +4859,7 @@
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C104" s="7">
         <v>0</v>
@@ -4927,72 +4924,72 @@
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C105" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="D105" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G105" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="H105" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E105" s="7" t="s">
+      <c r="I105" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="F105" s="8" t="s">
+      <c r="J105" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G105" s="15" t="s">
+      <c r="K105" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="L105" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="M105" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N105" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="O105" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="P105" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q105" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="H105" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="I105" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="J105" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="K105" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="L105" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="M105" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="N105" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="O105" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="P105" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q105" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="R105" s="1"/>
       <c r="S105" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T105" s="1"/>
       <c r="U105" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="V105" s="1"/>
       <c r="W105" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="X105" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C106" s="7" t="b">
         <v>0</v>
@@ -5057,78 +5054,72 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C107" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C107" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="D107" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G107" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H107" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I107" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J107" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K107" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L107" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M107" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N107" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O107" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P107" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="R107" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="R107" s="1"/>
       <c r="S107" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="T107" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="T107" s="1"/>
       <c r="U107" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="V107" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="V107" s="1"/>
       <c r="W107" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X107" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C108" s="7">
         <v>1.4</v>
@@ -5199,7 +5190,7 @@
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="8"/>
@@ -5226,7 +5217,7 @@
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C110" s="7">
         <v>0.01</v>
@@ -5281,7 +5272,7 @@
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C111" s="7">
         <v>4</v>
@@ -5340,7 +5331,7 @@
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="8"/>
@@ -5367,49 +5358,49 @@
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G113" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C113" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E113" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F113" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G113" s="15" t="s">
-        <v>149</v>
-      </c>
       <c r="H113" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I113" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J113" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K113" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L113" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M113" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N113" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O113" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P113" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
@@ -5418,15 +5409,15 @@
       <c r="U113" s="1"/>
       <c r="V113" s="1"/>
       <c r="W113" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X113" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C114" s="7">
         <v>10</v>
@@ -5473,7 +5464,7 @@
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C115" s="7">
         <v>0.7</v>
@@ -5532,7 +5523,7 @@
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C116" s="7">
         <v>1.2</v>
@@ -5591,7 +5582,7 @@
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C117" s="11">
         <v>40</v>

</xml_diff>